<commit_message>
Variable step time series update
</commit_message>
<xml_diff>
--- a/data/Input_data_multisample.xlsx
+++ b/data/Input_data_multisample.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustintharper/Documents/R/Utah/boron/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F10E08A4-7C1A-D441-9498-8439B5856C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4521C30-0D48-A941-8A00-51B2EC7E7D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="47420" yWindow="5060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="8">
   <si>
     <t>d11B</t>
   </si>
@@ -42,11 +55,14 @@
   <si>
     <t>d11Bsd</t>
   </si>
+  <si>
+    <t>Tsac</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -880,11 +896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1162,7 @@
         <v>4.34</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1226,7 +1242,7 @@
         <v>3.52</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>